<commit_message>
Updated BOM for 16mA fixed 470nm design.
</commit_message>
<xml_diff>
--- a/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
+++ b/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
@@ -152,7 +152,7 @@
     <t xml:space="preserve">R1</t>
   </si>
   <si>
-    <t xml:space="preserve">C854481</t>
+    <t xml:space="preserve">C413044</t>
   </si>
   <si>
     <t xml:space="preserve">30kΩ ±1%  Resistor</t>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changed 470nm LED due for 5V 16mA design due to footprint issue.
</commit_message>
<xml_diff>
--- a/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
+++ b/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">0603</t>
   </si>
   <si>
-    <t xml:space="preserve">C2962777</t>
+    <t xml:space="preserve">C434421</t>
   </si>
   <si>
     <t xml:space="preserve">4-Pin Connector, JST SM04B-SRSS-TB</t>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Modified BOM and CPLs of 470, 420, 557, 570, 660, 850 nm LEDs for new orders.
</commit_message>
<xml_diff>
--- a/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
+++ b/fixed/5V_regulator/470nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_470nm_16mA.xlsx
@@ -98,7 +98,7 @@
     <t xml:space="preserve">C3</t>
   </si>
   <si>
-    <t xml:space="preserve">C3012376</t>
+    <t xml:space="preserve">C1525</t>
   </si>
   <si>
     <t xml:space="preserve">LED (470nm)</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">SOT-23-5</t>
   </si>
   <si>
-    <t xml:space="preserve">C686637</t>
+    <t xml:space="preserve">C7972</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>